<commit_message>
Atualização Api, modificação nas scripts
</commit_message>
<xml_diff>
--- a/Modelagem/HROADS-Fisico.xlsx
+++ b/Modelagem/HROADS-Fisico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\SENAI\Desafio HROADS\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guica\Desktop\SENAI 2\HROADS_manha\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7320907A-0BC3-498A-8F29-DF73B8F80340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D94C17-9682-4AA2-A84F-34C5F016AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15360" yWindow="-2100" windowWidth="15375" windowHeight="7875" xr2:uid="{9EA8E97F-88A1-4632-BAAD-05E85D5AA331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{9EA8E97F-88A1-4632-BAAD-05E85D5AA331}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Personagem</t>
   </si>
@@ -139,13 +139,58 @@
   </si>
   <si>
     <t>ClasseHabilidade</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>nomeJogador</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>CardosinhoGameplay</t>
+  </si>
+  <si>
+    <t>cardoso@gmail.com</t>
+  </si>
+  <si>
+    <t>Ricardortc</t>
+  </si>
+  <si>
+    <t>ricardo@gmail.com</t>
+  </si>
+  <si>
+    <t>Sauloxiter</t>
+  </si>
+  <si>
+    <t>saulo@gmail.com</t>
+  </si>
+  <si>
+    <t>TipoUsuario</t>
+  </si>
+  <si>
+    <t>idTipoUsuario</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>Adm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +215,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -325,11 +378,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,6 +547,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,11 +589,35 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -771,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC46C1AD-5FA1-472E-8F62-8784FD703F7B}">
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,15 +942,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -899,17 +1060,17 @@
       <c r="I7" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -1030,7 +1191,7 @@
       <c r="B16" s="15">
         <v>6</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="29" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="2">
@@ -1095,15 +1256,15 @@
       <c r="H20" s="7"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="F22" s="29" t="s">
+      <c r="C22" s="34"/>
+      <c r="F22" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
@@ -1190,48 +1351,143 @@
       <c r="B28" s="1"/>
       <c r="E28" s="1"/>
     </row>
+    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="B30" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="G30" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="55"/>
+      <c r="I30" s="56"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
+      <c r="B31" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="46">
+        <v>1</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="48">
+        <v>1234</v>
+      </c>
+      <c r="G32" s="46">
+        <v>1</v>
+      </c>
+      <c r="H32" s="47">
+        <v>1</v>
+      </c>
+      <c r="I32" s="48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="46">
+        <v>2</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="48">
+        <v>12345</v>
+      </c>
+      <c r="G33" s="46">
+        <v>2</v>
+      </c>
+      <c r="H33" s="47">
+        <v>2</v>
+      </c>
+      <c r="I33" s="48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="50">
+        <v>3</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="53">
+        <v>123456</v>
+      </c>
+      <c r="G34" s="50">
+        <v>3</v>
+      </c>
+      <c r="H34" s="51">
+        <v>3</v>
+      </c>
+      <c r="I34" s="53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="G30:I30"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="F9:H9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D32" r:id="rId1" xr:uid="{D792A9A7-3710-4C10-8AE8-A26FB1580542}"/>
+    <hyperlink ref="D33" r:id="rId2" xr:uid="{1B021975-F6F8-450F-B215-C53B727B3708}"/>
+    <hyperlink ref="D34" r:id="rId3" xr:uid="{7742B2A8-5D9F-49AA-8518-13CC8572FEC0}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>